<commit_message>
Started moving Config Data into existing excel docs
</commit_message>
<xml_diff>
--- a/CI/TestSQL/02.TestData/CreatePledge.xlsx
+++ b/CI/TestSQL/02.TestData/CreatePledge.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Total_Pledge</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>User and Pledge Campaign must exist</t>
+  </si>
+  <si>
+    <t>mpcrds+cloudstrife@gmail.com</t>
+  </si>
+  <si>
+    <t>(t) GO Midgar 2018</t>
+  </si>
+  <si>
+    <t>First_Installment_Date</t>
   </si>
 </sst>
 </file>
@@ -104,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +433,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -432,7 +442,7 @@
     <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.46484375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
@@ -457,6 +467,9 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -471,6 +484,9 @@
       <c r="D2">
         <v>10</v>
       </c>
+      <c r="E2" s="1">
+        <v>43126</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -485,6 +501,9 @@
       <c r="D3">
         <v>10</v>
       </c>
+      <c r="E3" s="1">
+        <v>43126</v>
+      </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
@@ -502,6 +521,9 @@
       <c r="D4">
         <v>0</v>
       </c>
+      <c r="E4" s="1">
+        <v>43126</v>
+      </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
@@ -519,8 +541,26 @@
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5" s="1">
+        <v>43126</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43101</v>
+      </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>

</xml_diff>